<commit_message>
updated taxable excel sheet.
</commit_message>
<xml_diff>
--- a/DividendLiberty/Taxable.xlsx
+++ b/DividendLiberty/Taxable.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve Yi\Documents\GitHub\DividendLibertyCommercial\DividendLiberty\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve Yi\Documents\GitHub\DividendLibertyCommercial\DividendLiberty\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12570" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12570" windowHeight="11985" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Buys" sheetId="3" r:id="rId1"/>
@@ -659,7 +659,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BP148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
@@ -3033,8 +3033,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:V23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated taxable excel and xml for taxable account.
</commit_message>
<xml_diff>
--- a/DividendLiberty/Taxable.xlsx
+++ b/DividendLiberty/Taxable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12576" windowHeight="11988" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12570" windowHeight="11985" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Buys" sheetId="3" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="2016" sheetId="2" r:id="rId3"/>
     <sheet name="2017" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="69">
   <si>
     <t>Symbols</t>
   </si>
@@ -217,11 +217,29 @@
   <si>
     <t>buy</t>
   </si>
+  <si>
+    <t>CHD</t>
+  </si>
+  <si>
+    <t>MKC</t>
+  </si>
+  <si>
+    <t>SJM</t>
+  </si>
+  <si>
+    <t>McCormick &amp; Company Inc</t>
+  </si>
+  <si>
+    <t>Church &amp; Dwight Co</t>
+  </si>
+  <si>
+    <t>J M Smucker Co</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
@@ -269,7 +287,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,6 +342,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -337,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -376,6 +400,12 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="2" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,23 +499,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -521,23 +534,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -691,62 +687,62 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:BP148"/>
+  <dimension ref="A1:BP200"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="V86" sqref="V86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.33203125" customWidth="1"/>
-    <col min="22" max="22" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.28515625" customWidth="1"/>
+    <col min="22" max="22" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7" customWidth="1"/>
-    <col min="25" max="25" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.5546875" customWidth="1"/>
-    <col min="28" max="28" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.109375" customWidth="1"/>
-    <col min="31" max="31" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.44140625" customWidth="1"/>
-    <col min="34" max="34" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.5703125" customWidth="1"/>
+    <col min="28" max="28" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.140625" customWidth="1"/>
+    <col min="31" max="31" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.42578125" customWidth="1"/>
+    <col min="34" max="34" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -819,7 +815,7 @@
       <c r="BO1" s="3"/>
       <c r="BP1" s="2"/>
     </row>
-    <row r="2" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>42272</v>
       </c>
@@ -913,7 +909,7 @@
       <c r="BO2" s="4"/>
       <c r="BP2" s="17"/>
     </row>
-    <row r="3" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:68" x14ac:dyDescent="0.25">
       <c r="D3" s="4">
         <v>42612</v>
       </c>
@@ -922,73 +918,73 @@
       </c>
       <c r="Z3" s="17"/>
     </row>
-    <row r="15" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="25"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="25"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="25"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="25"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="25"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="25"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="25"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="25"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="25"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="25"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="25"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="25"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="25"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="25"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" s="25"/>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B33" s="25"/>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B34" s="25"/>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B35" s="25"/>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B36" s="25"/>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B37" s="25"/>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B38" s="25"/>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B40" s="17"/>
       <c r="E40" s="17"/>
       <c r="H40" s="17"/>
@@ -1000,7 +996,7 @@
       <c r="Z40" s="17"/>
       <c r="AC40" s="17"/>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>58</v>
       </c>
@@ -1045,7 +1041,7 @@
         <v>989.4</v>
       </c>
     </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>12</v>
       </c>
@@ -1107,7 +1103,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>42268</v>
       </c>
@@ -1199,7 +1195,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>42612</v>
       </c>
@@ -1255,7 +1251,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B53" s="29"/>
       <c r="K53" s="29"/>
       <c r="Q53" s="29"/>
@@ -1271,7 +1267,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B54" s="29"/>
       <c r="K54" s="29"/>
       <c r="Q54" s="29"/>
@@ -1287,308 +1283,308 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B55" s="29"/>
       <c r="K55" s="29"/>
       <c r="Q55" s="29"/>
       <c r="W55" s="29"/>
       <c r="Z55" s="29"/>
     </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B56" s="29"/>
       <c r="K56" s="29"/>
       <c r="Q56" s="29"/>
       <c r="W56" s="29"/>
       <c r="Z56" s="29"/>
     </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B57" s="29"/>
       <c r="K57" s="29"/>
       <c r="Q57" s="29"/>
       <c r="W57" s="29"/>
       <c r="Z57" s="29"/>
     </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B58" s="29"/>
       <c r="K58" s="29"/>
       <c r="Q58" s="29"/>
       <c r="W58" s="29"/>
       <c r="Z58" s="29"/>
     </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B59" s="29"/>
       <c r="K59" s="29"/>
       <c r="Q59" s="29"/>
       <c r="W59" s="29"/>
       <c r="Z59" s="29"/>
     </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B60" s="29"/>
       <c r="K60" s="29"/>
       <c r="Q60" s="29"/>
       <c r="W60" s="29"/>
       <c r="Z60" s="29"/>
     </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B61" s="29"/>
       <c r="K61" s="29"/>
       <c r="Q61" s="29"/>
       <c r="W61" s="29"/>
       <c r="Z61" s="29"/>
     </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B62" s="29"/>
       <c r="K62" s="29"/>
       <c r="Q62" s="29"/>
       <c r="W62" s="29"/>
       <c r="Z62" s="29"/>
     </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B63" s="29"/>
       <c r="K63" s="29"/>
       <c r="Q63" s="29"/>
       <c r="W63" s="29"/>
       <c r="Z63" s="29"/>
     </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B64" s="29"/>
       <c r="K64" s="29"/>
       <c r="Q64" s="29"/>
       <c r="W64" s="29"/>
       <c r="Z64" s="29"/>
     </row>
-    <row r="65" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B65" s="29"/>
       <c r="K65" s="29"/>
       <c r="Q65" s="29"/>
       <c r="W65" s="29"/>
       <c r="Z65" s="29"/>
     </row>
-    <row r="66" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B66" s="29"/>
       <c r="K66" s="29"/>
       <c r="Q66" s="29"/>
       <c r="W66" s="29"/>
       <c r="Z66" s="29"/>
     </row>
-    <row r="67" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B67" s="29"/>
       <c r="K67" s="29"/>
       <c r="Q67" s="29"/>
       <c r="W67" s="29"/>
       <c r="Z67" s="29"/>
     </row>
-    <row r="68" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B68" s="29"/>
       <c r="K68" s="29"/>
       <c r="Q68" s="29"/>
       <c r="W68" s="29"/>
       <c r="Z68" s="29"/>
     </row>
-    <row r="69" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B69" s="29"/>
       <c r="K69" s="29"/>
       <c r="Q69" s="29"/>
       <c r="W69" s="29"/>
       <c r="Z69" s="29"/>
     </row>
-    <row r="70" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B70" s="29"/>
       <c r="K70" s="29"/>
       <c r="Q70" s="29"/>
       <c r="W70" s="29"/>
       <c r="Z70" s="29"/>
     </row>
-    <row r="71" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B71" s="29"/>
       <c r="K71" s="29"/>
       <c r="Q71" s="29"/>
       <c r="W71" s="29"/>
       <c r="Z71" s="29"/>
     </row>
-    <row r="72" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B72" s="29"/>
       <c r="K72" s="29"/>
       <c r="Q72" s="29"/>
       <c r="W72" s="29"/>
       <c r="Z72" s="29"/>
     </row>
-    <row r="73" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B73" s="29"/>
       <c r="K73" s="29"/>
       <c r="Q73" s="29"/>
       <c r="W73" s="29"/>
       <c r="Z73" s="29"/>
     </row>
-    <row r="74" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B74" s="29"/>
       <c r="K74" s="29"/>
       <c r="Q74" s="29"/>
       <c r="W74" s="29"/>
       <c r="Z74" s="29"/>
     </row>
-    <row r="75" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B75" s="29"/>
       <c r="K75" s="29"/>
       <c r="Q75" s="29"/>
       <c r="W75" s="29"/>
       <c r="Z75" s="29"/>
     </row>
-    <row r="76" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B76" s="29"/>
       <c r="K76" s="29"/>
       <c r="Q76" s="29"/>
       <c r="W76" s="29"/>
       <c r="Z76" s="29"/>
     </row>
-    <row r="77" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B77" s="29"/>
       <c r="K77" s="29"/>
       <c r="Q77" s="29"/>
       <c r="W77" s="29"/>
       <c r="Z77" s="29"/>
     </row>
-    <row r="78" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B78" s="29"/>
       <c r="K78" s="29"/>
       <c r="Q78" s="29"/>
       <c r="W78" s="29"/>
       <c r="Z78" s="29"/>
     </row>
-    <row r="79" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B79" s="29"/>
       <c r="K79" s="29"/>
       <c r="Q79" s="29"/>
       <c r="W79" s="29"/>
       <c r="Z79" s="29"/>
     </row>
-    <row r="80" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B80" s="29"/>
       <c r="K80" s="29"/>
       <c r="Q80" s="29"/>
       <c r="W80" s="29"/>
       <c r="Z80" s="29"/>
     </row>
-    <row r="81" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B81" s="29"/>
       <c r="K81" s="29"/>
       <c r="Q81" s="29"/>
       <c r="W81" s="29"/>
       <c r="Z81" s="29"/>
     </row>
-    <row r="82" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B82" s="29"/>
       <c r="K82" s="29"/>
       <c r="Q82" s="29"/>
       <c r="W82" s="29"/>
       <c r="Z82" s="29"/>
     </row>
-    <row r="83" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B83" s="29"/>
       <c r="K83" s="29"/>
       <c r="Q83" s="29"/>
       <c r="W83" s="29"/>
       <c r="Z83" s="29"/>
     </row>
-    <row r="84" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B84" s="29"/>
       <c r="K84" s="29"/>
       <c r="Q84" s="29"/>
       <c r="W84" s="29"/>
       <c r="Z84" s="29"/>
     </row>
-    <row r="85" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B85" s="29"/>
       <c r="K85" s="29"/>
       <c r="Q85" s="29"/>
       <c r="W85" s="29"/>
       <c r="Z85" s="29"/>
     </row>
-    <row r="86" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B86" s="29"/>
       <c r="K86" s="29"/>
       <c r="Q86" s="29"/>
       <c r="W86" s="29"/>
       <c r="Z86" s="29"/>
     </row>
-    <row r="87" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B87" s="29"/>
       <c r="K87" s="29"/>
       <c r="Q87" s="29"/>
       <c r="W87" s="29"/>
       <c r="Z87" s="29"/>
     </row>
-    <row r="88" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B88" s="29"/>
       <c r="K88" s="29"/>
       <c r="Q88" s="29"/>
       <c r="W88" s="29"/>
       <c r="Z88" s="29"/>
     </row>
-    <row r="89" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B89" s="29"/>
       <c r="K89" s="29"/>
       <c r="Q89" s="29"/>
       <c r="W89" s="29"/>
       <c r="Z89" s="29"/>
     </row>
-    <row r="90" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B90" s="29"/>
       <c r="K90" s="29"/>
       <c r="Q90" s="29"/>
       <c r="W90" s="29"/>
       <c r="Z90" s="29"/>
     </row>
-    <row r="91" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B91" s="29"/>
       <c r="K91" s="29"/>
       <c r="Q91" s="29"/>
       <c r="W91" s="29"/>
       <c r="Z91" s="29"/>
     </row>
-    <row r="92" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B92" s="29"/>
       <c r="K92" s="29"/>
       <c r="Q92" s="29"/>
       <c r="W92" s="29"/>
       <c r="Z92" s="29"/>
     </row>
-    <row r="93" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B93" s="29"/>
       <c r="K93" s="29"/>
       <c r="Q93" s="29"/>
       <c r="W93" s="29"/>
       <c r="Z93" s="29"/>
     </row>
-    <row r="94" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B94" s="29"/>
       <c r="K94" s="29"/>
       <c r="Q94" s="29"/>
       <c r="W94" s="29"/>
       <c r="Z94" s="29"/>
     </row>
-    <row r="95" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B95" s="29"/>
       <c r="K95" s="29"/>
       <c r="Q95" s="29"/>
       <c r="W95" s="29"/>
       <c r="Z95" s="29"/>
     </row>
-    <row r="96" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B96" s="29"/>
       <c r="K96" s="29"/>
       <c r="Q96" s="29"/>
       <c r="W96" s="29"/>
       <c r="Z96" s="29"/>
     </row>
-    <row r="97" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B97" s="29"/>
       <c r="K97" s="29"/>
       <c r="Q97" s="29"/>
       <c r="W97" s="29"/>
       <c r="Z97" s="29"/>
     </row>
-    <row r="98" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B98" s="17">
         <f>SUM(B51:B97)</f>
         <v>2951.1000000000004</v>
@@ -1630,7 +1626,7 @@
         <v>1916.7600000000002</v>
       </c>
     </row>
-    <row r="100" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>12</v>
       </c>
@@ -1638,7 +1634,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="101" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>42268</v>
       </c>
@@ -1649,7 +1645,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="102" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>42612</v>
       </c>
@@ -1660,145 +1656,207 @@
         <v>62</v>
       </c>
     </row>
-    <row r="103" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B103" s="29"/>
     </row>
-    <row r="104" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B104" s="29"/>
     </row>
-    <row r="105" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B105" s="29"/>
     </row>
-    <row r="106" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B106" s="29"/>
     </row>
-    <row r="107" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B107" s="29"/>
     </row>
-    <row r="108" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B108" s="29"/>
     </row>
-    <row r="109" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B109" s="29"/>
     </row>
-    <row r="110" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B110" s="29"/>
     </row>
-    <row r="111" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B111" s="29"/>
     </row>
-    <row r="112" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B112" s="29"/>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B113" s="29"/>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B114" s="29"/>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" s="29"/>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" s="29"/>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" s="29"/>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B118" s="29"/>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B119" s="29"/>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" s="29"/>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B121" s="29"/>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" s="29"/>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B123" s="29"/>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B124" s="29"/>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B125" s="29"/>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B126" s="29"/>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B127" s="29"/>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B128" s="29"/>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B129" s="29"/>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B130" s="29"/>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B131" s="29"/>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B132" s="29"/>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B133" s="29"/>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B134" s="29"/>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B135" s="29"/>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B136" s="29"/>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B137" s="29"/>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B138" s="29"/>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B139" s="29"/>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B140" s="29"/>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B141" s="29"/>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B142" s="29"/>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B143" s="29"/>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B144" s="29"/>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B145" s="29"/>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B146" s="29"/>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B147" s="29"/>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B148" s="17">
         <f>SUM(B101:B147)</f>
         <v>1988.76</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A150" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B150" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E150" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G150" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H150" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A151" s="4">
+        <v>42667</v>
+      </c>
+      <c r="B151" s="17">
+        <v>2042.5</v>
+      </c>
+      <c r="D151" s="4">
+        <v>42667</v>
+      </c>
+      <c r="E151" s="17">
+        <v>1412.7</v>
+      </c>
+      <c r="G151" s="4">
+        <v>42667</v>
+      </c>
+      <c r="H151" s="17">
+        <v>1303.4000000000001</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A152" s="4"/>
+      <c r="B152" s="29"/>
+      <c r="D152" s="4"/>
+      <c r="E152" s="29"/>
+      <c r="G152" s="4"/>
+      <c r="H152" s="29"/>
+    </row>
+    <row r="200" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B200" s="29">
+        <f>SUM(B151,B199)</f>
+        <v>2042.5</v>
+      </c>
+      <c r="E200" s="29">
+        <f>SUM(E151,E199)</f>
+        <v>1412.7</v>
+      </c>
+      <c r="H200" s="29">
+        <f>SUM(H151,H199)</f>
+        <v>1303.4000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1816,31 +1874,31 @@
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1902,7 +1960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
@@ -1967,7 +2025,7 @@
         <v>1025.99</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
@@ -2032,7 +2090,7 @@
         <v>1039.2</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>23</v>
       </c>
@@ -2097,7 +2155,7 @@
         <v>1019.5200000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
@@ -2162,7 +2220,7 @@
         <v>1087.3500000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>25</v>
       </c>
@@ -2227,7 +2285,7 @@
         <v>1012.94</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>26</v>
       </c>
@@ -2292,7 +2350,7 @@
         <v>929.86</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>7</v>
       </c>
@@ -2357,7 +2415,7 @@
         <v>1007.49</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
@@ -2422,7 +2480,7 @@
         <v>1032.78</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>28</v>
       </c>
@@ -2487,7 +2545,7 @@
         <v>994.15</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
@@ -2552,7 +2610,7 @@
         <v>1048.5800000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>17</v>
       </c>
@@ -2617,7 +2675,7 @@
         <v>871.18</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>29</v>
       </c>
@@ -2682,7 +2740,7 @@
         <v>985.64</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>32</v>
       </c>
@@ -2747,7 +2805,7 @@
         <v>1954.8</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>33</v>
       </c>
@@ -2812,7 +2870,7 @@
         <v>974.44</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>34</v>
       </c>
@@ -2877,7 +2935,7 @@
         <v>986.35</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>37</v>
       </c>
@@ -2942,7 +3000,7 @@
         <v>1023.2</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>38</v>
       </c>
@@ -3007,7 +3065,7 @@
         <v>1033.8599999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="26"/>
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
@@ -3080,35 +3138,35 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:V23"/>
+  <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -3176,7 +3234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>16</v>
       </c>
@@ -3190,7 +3248,7 @@
         <v>24.728000000000002</v>
       </c>
       <c r="E2" s="20">
-        <f t="shared" ref="E2:E22" si="0">V2/D2</f>
+        <f t="shared" ref="E2:E25" si="0">V2/D2</f>
         <v>42.377062439340008</v>
       </c>
       <c r="F2" s="6">
@@ -3238,19 +3296,19 @@
         <v>0</v>
       </c>
       <c r="T2" s="15">
-        <f t="shared" ref="T2:T22" si="1">SUM(H2:S2)</f>
+        <f t="shared" ref="T2:T25" si="1">SUM(H2:S2)</f>
         <v>21.909999999999997</v>
       </c>
       <c r="U2" s="15">
-        <f t="shared" ref="U2:U22" si="2">SUM(G2:S2)</f>
+        <f t="shared" ref="U2:U25" si="2">SUM(G2:S2)</f>
         <v>28.619999999999997</v>
       </c>
       <c r="V2" s="13">
-        <f t="shared" ref="V2:V22" si="3">SUM(F2, U2)</f>
+        <f t="shared" ref="V2:V25" si="3">SUM(F2, U2)</f>
         <v>1047.8999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>21</v>
       </c>
@@ -3323,7 +3381,7 @@
         <v>1853.59</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>22</v>
       </c>
@@ -3337,7 +3395,7 @@
         <v>16.690000000000001</v>
       </c>
       <c r="E4" s="20">
-        <f t="shared" si="0"/>
+        <f>V4/D4</f>
         <v>64.525464349910123</v>
       </c>
       <c r="F4" s="6">
@@ -3397,1405 +3455,1624 @@
         <v>1076.93</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="31" t="s">
+    <row r="5" spans="1:22" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="32">
+        <v>43</v>
+      </c>
+      <c r="E5" s="34">
+        <f>V5/D5</f>
+        <v>47.5</v>
+      </c>
+      <c r="F5" s="35">
+        <f>'Initial Buys'!B200</f>
+        <v>2042.5</v>
+      </c>
+      <c r="G5" s="36">
+        <v>0</v>
+      </c>
+      <c r="H5" s="22">
+        <v>0</v>
+      </c>
+      <c r="I5" s="21">
+        <v>0</v>
+      </c>
+      <c r="J5" s="22">
+        <v>0</v>
+      </c>
+      <c r="K5" s="21">
+        <v>0</v>
+      </c>
+      <c r="L5" s="22">
+        <v>0</v>
+      </c>
+      <c r="M5" s="21">
+        <v>0</v>
+      </c>
+      <c r="N5" s="22">
+        <v>0</v>
+      </c>
+      <c r="O5" s="21">
+        <v>0</v>
+      </c>
+      <c r="P5" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="21">
+        <v>0</v>
+      </c>
+      <c r="R5" s="22">
+        <v>0</v>
+      </c>
+      <c r="S5" s="21">
+        <v>0</v>
+      </c>
+      <c r="T5" s="36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U5" s="36">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V5" s="37">
+        <f t="shared" si="3"/>
+        <v>2042.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B6" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D6" s="5">
         <v>16.358000000000001</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E6" s="20">
         <f t="shared" si="0"/>
         <v>63.470473162978358</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F6" s="6">
         <f>'Initial Buys'!K48</f>
         <v>1013.44</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G6" s="15">
         <f>'2015'!S4</f>
         <v>6.08</v>
       </c>
-      <c r="H5" s="22">
-        <v>0</v>
-      </c>
-      <c r="I5" s="21">
+      <c r="H6" s="22">
+        <v>0</v>
+      </c>
+      <c r="I6" s="21">
         <v>6.09</v>
       </c>
-      <c r="J5" s="22">
-        <v>0</v>
-      </c>
-      <c r="K5" s="21">
-        <v>0</v>
-      </c>
-      <c r="L5" s="22">
+      <c r="J6" s="22">
+        <v>0</v>
+      </c>
+      <c r="K6" s="21">
+        <v>0</v>
+      </c>
+      <c r="L6" s="22">
         <v>6.31</v>
       </c>
-      <c r="M5" s="21">
-        <v>0</v>
-      </c>
-      <c r="N5" s="22">
-        <v>0</v>
-      </c>
-      <c r="O5" s="21">
+      <c r="M6" s="21">
+        <v>0</v>
+      </c>
+      <c r="N6" s="22">
+        <v>0</v>
+      </c>
+      <c r="O6" s="21">
         <v>6.33</v>
       </c>
-      <c r="P5" s="22">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="21">
-        <v>0</v>
-      </c>
-      <c r="R5" s="22">
-        <v>0</v>
-      </c>
-      <c r="S5" s="21">
-        <v>0</v>
-      </c>
-      <c r="T5" s="14">
+      <c r="P6" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="21">
+        <v>0</v>
+      </c>
+      <c r="R6" s="22">
+        <v>0</v>
+      </c>
+      <c r="S6" s="21">
+        <v>0</v>
+      </c>
+      <c r="T6" s="15">
         <f t="shared" si="1"/>
         <v>18.729999999999997</v>
       </c>
-      <c r="U5" s="14">
+      <c r="U6" s="15">
         <f t="shared" si="2"/>
         <v>24.810000000000002</v>
       </c>
-      <c r="V5" s="12">
+      <c r="V6" s="13">
         <f t="shared" si="3"/>
         <v>1038.25</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A6" s="30" t="s">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B7" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C7" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D7" s="32">
         <v>14.637</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E7" s="34">
         <f t="shared" si="0"/>
         <v>77.426385188221644</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F7" s="35">
         <f>'Initial Buys'!N48</f>
         <v>1072.4000000000001</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G7" s="36">
         <f>'2015'!S5</f>
         <v>14.95</v>
       </c>
-      <c r="H6" s="22">
-        <v>0</v>
-      </c>
-      <c r="I6" s="21">
-        <v>0</v>
-      </c>
-      <c r="J6" s="22">
+      <c r="H7" s="22">
+        <v>0</v>
+      </c>
+      <c r="I7" s="21">
+        <v>0</v>
+      </c>
+      <c r="J7" s="22">
         <v>15.13</v>
       </c>
-      <c r="K6" s="21">
-        <v>0</v>
-      </c>
-      <c r="L6" s="22">
-        <v>0</v>
-      </c>
-      <c r="M6" s="21">
+      <c r="K7" s="21">
+        <v>0</v>
+      </c>
+      <c r="L7" s="22">
+        <v>0</v>
+      </c>
+      <c r="M7" s="21">
         <v>15.34</v>
       </c>
-      <c r="N6" s="22">
-        <v>0</v>
-      </c>
-      <c r="O6" s="21">
-        <v>0</v>
-      </c>
-      <c r="P6" s="22">
+      <c r="N7" s="22">
+        <v>0</v>
+      </c>
+      <c r="O7" s="21">
+        <v>0</v>
+      </c>
+      <c r="P7" s="22">
         <v>15.47</v>
       </c>
-      <c r="Q6" s="21">
-        <v>0</v>
-      </c>
-      <c r="R6" s="22">
-        <v>0</v>
-      </c>
-      <c r="S6" s="21">
-        <v>0</v>
-      </c>
-      <c r="T6" s="15">
+      <c r="Q7" s="21">
+        <v>0</v>
+      </c>
+      <c r="R7" s="22">
+        <v>0</v>
+      </c>
+      <c r="S7" s="21">
+        <v>0</v>
+      </c>
+      <c r="T7" s="36">
         <f t="shared" si="1"/>
         <v>45.94</v>
       </c>
-      <c r="U6" s="15">
+      <c r="U7" s="36">
         <f t="shared" si="2"/>
         <v>60.89</v>
       </c>
-      <c r="V6" s="13">
+      <c r="V7" s="37">
         <f t="shared" si="3"/>
         <v>1133.2900000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A7" s="31" t="s">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B8" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D8" s="5">
         <v>14.324999999999999</v>
       </c>
-      <c r="E7" s="19">
-        <f>V7/D7</f>
+      <c r="E8" s="20">
+        <f>V8/D8</f>
         <v>72.484467713787097</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F8" s="6">
         <f>'Initial Buys'!Q48</f>
         <v>1012.94</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G8" s="15">
         <f>'2015'!S6</f>
         <v>0</v>
       </c>
-      <c r="H7" s="22">
-        <v>0</v>
-      </c>
-      <c r="I7" s="21">
+      <c r="H8" s="22">
+        <v>0</v>
+      </c>
+      <c r="I8" s="21">
         <v>8.4</v>
       </c>
-      <c r="J7" s="22">
-        <v>0</v>
-      </c>
-      <c r="K7" s="21">
-        <v>0</v>
-      </c>
-      <c r="L7" s="22">
+      <c r="J8" s="22">
+        <v>0</v>
+      </c>
+      <c r="K8" s="21">
+        <v>0</v>
+      </c>
+      <c r="L8" s="22">
         <v>8.4700000000000006</v>
       </c>
-      <c r="M7" s="21">
-        <v>0</v>
-      </c>
-      <c r="N7" s="22">
-        <v>0</v>
-      </c>
-      <c r="O7" s="21">
+      <c r="M8" s="21">
+        <v>0</v>
+      </c>
+      <c r="N8" s="22">
+        <v>0</v>
+      </c>
+      <c r="O8" s="21">
         <v>8.5299999999999994</v>
       </c>
-      <c r="P7" s="22">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="21">
-        <v>0</v>
-      </c>
-      <c r="R7" s="22">
-        <v>0</v>
-      </c>
-      <c r="S7" s="21">
-        <v>0</v>
-      </c>
-      <c r="T7" s="14">
+      <c r="P8" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="21">
+        <v>0</v>
+      </c>
+      <c r="R8" s="22">
+        <v>0</v>
+      </c>
+      <c r="S8" s="21">
+        <v>0</v>
+      </c>
+      <c r="T8" s="15">
         <f t="shared" si="1"/>
         <v>25.4</v>
       </c>
-      <c r="U7" s="14">
+      <c r="U8" s="15">
         <f t="shared" si="2"/>
         <v>25.4</v>
       </c>
-      <c r="V7" s="12">
+      <c r="V8" s="13">
         <f t="shared" si="3"/>
         <v>1038.3400000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A8" s="30" t="s">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B9" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C9" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D9" s="32">
         <v>14.522</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E9" s="34">
         <f t="shared" si="0"/>
         <v>66.001928109075891</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F9" s="35">
         <f>'Initial Buys'!T48</f>
         <v>920.78</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G9" s="36">
         <f>'2015'!S7</f>
         <v>9.08</v>
       </c>
-      <c r="H8" s="22">
-        <v>0</v>
-      </c>
-      <c r="I8" s="21">
-        <v>0</v>
-      </c>
-      <c r="J8" s="22">
+      <c r="H9" s="22">
+        <v>0</v>
+      </c>
+      <c r="I9" s="21">
+        <v>0</v>
+      </c>
+      <c r="J9" s="22">
         <v>9.5</v>
       </c>
-      <c r="K8" s="21">
-        <v>0</v>
-      </c>
-      <c r="L8" s="22">
-        <v>0</v>
-      </c>
-      <c r="M8" s="21">
+      <c r="K9" s="21">
+        <v>0</v>
+      </c>
+      <c r="L9" s="22">
+        <v>0</v>
+      </c>
+      <c r="M9" s="21">
         <v>9.52</v>
       </c>
-      <c r="N8" s="22">
-        <v>0</v>
-      </c>
-      <c r="O8" s="21">
-        <v>0</v>
-      </c>
-      <c r="P8" s="22">
+      <c r="N9" s="22">
+        <v>0</v>
+      </c>
+      <c r="O9" s="21">
+        <v>0</v>
+      </c>
+      <c r="P9" s="22">
         <v>9.6</v>
       </c>
-      <c r="Q8" s="21">
-        <v>0</v>
-      </c>
-      <c r="R8" s="22">
-        <v>0</v>
-      </c>
-      <c r="S8" s="21">
-        <v>0</v>
-      </c>
-      <c r="T8" s="15">
+      <c r="Q9" s="21">
+        <v>0</v>
+      </c>
+      <c r="R9" s="22">
+        <v>0</v>
+      </c>
+      <c r="S9" s="21">
+        <v>0</v>
+      </c>
+      <c r="T9" s="36">
         <f t="shared" si="1"/>
         <v>28.619999999999997</v>
       </c>
-      <c r="U8" s="15">
+      <c r="U9" s="36">
         <f t="shared" si="2"/>
         <v>37.699999999999996</v>
       </c>
-      <c r="V8" s="13">
+      <c r="V9" s="37">
         <f t="shared" si="3"/>
         <v>958.48</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A9" s="31" t="s">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D10" s="5">
         <v>22.847000000000001</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E10" s="20">
         <f t="shared" si="0"/>
         <v>45.495688711865888</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F10" s="6">
         <f>'Initial Buys'!W48</f>
         <v>997.04</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G10" s="15">
         <f>'2015'!S8</f>
         <v>10.45</v>
       </c>
-      <c r="H9" s="22">
-        <v>0</v>
-      </c>
-      <c r="I9" s="21">
-        <v>0</v>
-      </c>
-      <c r="J9" s="22">
+      <c r="H10" s="22">
+        <v>0</v>
+      </c>
+      <c r="I10" s="21">
+        <v>0</v>
+      </c>
+      <c r="J10" s="22">
         <v>10.54</v>
       </c>
-      <c r="K9" s="21">
-        <v>0</v>
-      </c>
-      <c r="L9" s="22">
-        <v>0</v>
-      </c>
-      <c r="M9" s="21">
+      <c r="K10" s="21">
+        <v>0</v>
+      </c>
+      <c r="L10" s="22">
+        <v>0</v>
+      </c>
+      <c r="M10" s="21">
         <v>10.66</v>
       </c>
-      <c r="N9" s="22">
-        <v>0</v>
-      </c>
-      <c r="O9" s="21">
-        <v>0</v>
-      </c>
-      <c r="P9" s="22">
+      <c r="N10" s="22">
+        <v>0</v>
+      </c>
+      <c r="O10" s="21">
+        <v>0</v>
+      </c>
+      <c r="P10" s="22">
         <v>10.75</v>
       </c>
-      <c r="Q9" s="21">
-        <v>0</v>
-      </c>
-      <c r="R9" s="22">
-        <v>0</v>
-      </c>
-      <c r="S9" s="21">
-        <v>0</v>
-      </c>
-      <c r="T9" s="14">
+      <c r="Q10" s="21">
+        <v>0</v>
+      </c>
+      <c r="R10" s="22">
+        <v>0</v>
+      </c>
+      <c r="S10" s="21">
+        <v>0</v>
+      </c>
+      <c r="T10" s="15">
         <f t="shared" si="1"/>
         <v>31.95</v>
       </c>
-      <c r="U9" s="14">
+      <c r="U10" s="15">
         <f t="shared" si="2"/>
         <v>42.4</v>
       </c>
-      <c r="V9" s="12">
+      <c r="V10" s="13">
         <f t="shared" si="3"/>
         <v>1039.44</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A10" s="30" t="s">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B11" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C11" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D11" s="32">
         <v>18.501999999999999</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E11" s="34">
         <f t="shared" si="0"/>
         <v>57.179764349800017</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F11" s="35">
         <f>'Initial Buys'!Z48</f>
         <v>1027.08</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G11" s="36">
         <f>'2015'!S9</f>
         <v>5.7</v>
       </c>
-      <c r="H10" s="22">
-        <v>0</v>
-      </c>
-      <c r="I10" s="21">
+      <c r="H11" s="22">
+        <v>0</v>
+      </c>
+      <c r="I11" s="21">
         <v>7.96</v>
       </c>
-      <c r="J10" s="22">
-        <v>0</v>
-      </c>
-      <c r="K10" s="21">
-        <v>0</v>
-      </c>
-      <c r="L10" s="22">
+      <c r="J11" s="22">
+        <v>0</v>
+      </c>
+      <c r="K11" s="21">
+        <v>0</v>
+      </c>
+      <c r="L11" s="22">
         <v>8.39</v>
       </c>
-      <c r="M10" s="21">
-        <v>0</v>
-      </c>
-      <c r="N10" s="22">
-        <v>0</v>
-      </c>
-      <c r="O10" s="21">
+      <c r="M11" s="21">
+        <v>0</v>
+      </c>
+      <c r="N11" s="22">
+        <v>0</v>
+      </c>
+      <c r="O11" s="21">
         <v>8.81</v>
       </c>
-      <c r="P10" s="22">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="21">
-        <v>0</v>
-      </c>
-      <c r="R10" s="22">
-        <v>0</v>
-      </c>
-      <c r="S10" s="21">
-        <v>0</v>
-      </c>
-      <c r="T10" s="15">
+      <c r="P11" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="21">
+        <v>0</v>
+      </c>
+      <c r="R11" s="22">
+        <v>0</v>
+      </c>
+      <c r="S11" s="21">
+        <v>0</v>
+      </c>
+      <c r="T11" s="36">
         <f t="shared" si="1"/>
         <v>25.160000000000004</v>
       </c>
-      <c r="U10" s="15">
+      <c r="U11" s="36">
         <f t="shared" si="2"/>
         <v>30.86</v>
       </c>
-      <c r="V10" s="13">
+      <c r="V11" s="37">
         <f t="shared" si="3"/>
         <v>1057.9399999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A11" s="31" t="s">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B12" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D12" s="5">
         <v>12.327</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E12" s="20">
         <f t="shared" si="0"/>
         <v>82.91717368378356</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F12" s="6">
         <f>'Initial Buys'!AC48</f>
         <v>989.4</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G12" s="15">
         <f>'2015'!S10</f>
         <v>4.75</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H12" s="22">
         <v>6.63</v>
       </c>
-      <c r="I11" s="21">
-        <v>0</v>
-      </c>
-      <c r="J11" s="22">
-        <v>0</v>
-      </c>
-      <c r="K11" s="21">
+      <c r="I12" s="21">
+        <v>0</v>
+      </c>
+      <c r="J12" s="22">
+        <v>0</v>
+      </c>
+      <c r="K12" s="21">
         <v>6.66</v>
       </c>
-      <c r="L11" s="22">
-        <v>0</v>
-      </c>
-      <c r="M11" s="21">
-        <v>0</v>
-      </c>
-      <c r="N11" s="22">
+      <c r="L12" s="22">
+        <v>0</v>
+      </c>
+      <c r="M12" s="21">
+        <v>0</v>
+      </c>
+      <c r="N12" s="22">
         <v>6.71</v>
       </c>
-      <c r="O11" s="21">
-        <v>0</v>
-      </c>
-      <c r="P11" s="22">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="21">
+      <c r="O12" s="21">
+        <v>0</v>
+      </c>
+      <c r="P12" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="21">
         <v>7.97</v>
       </c>
-      <c r="R11" s="22">
-        <v>0</v>
-      </c>
-      <c r="S11" s="21">
-        <v>0</v>
-      </c>
-      <c r="T11" s="14">
+      <c r="R12" s="22">
+        <v>0</v>
+      </c>
+      <c r="S12" s="21">
+        <v>0</v>
+      </c>
+      <c r="T12" s="15">
         <f t="shared" si="1"/>
         <v>27.97</v>
       </c>
-      <c r="U11" s="14">
+      <c r="U12" s="15">
         <f t="shared" si="2"/>
         <v>32.72</v>
       </c>
-      <c r="V11" s="12">
+      <c r="V12" s="13">
         <f t="shared" si="3"/>
         <v>1022.12</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A12" s="30" t="s">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B13" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C13" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D13" s="32">
         <v>27.31</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E13" s="34">
         <f t="shared" si="0"/>
         <v>109.31819846210182</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F13" s="35">
         <f>'Initial Buys'!B98</f>
         <v>2951.1000000000004</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G13" s="36">
         <f>'2015'!S11</f>
         <v>8.1999999999999993</v>
       </c>
-      <c r="H12" s="22">
-        <v>0</v>
-      </c>
-      <c r="I12" s="21">
-        <v>0</v>
-      </c>
-      <c r="J12" s="22">
+      <c r="H13" s="22">
+        <v>0</v>
+      </c>
+      <c r="I13" s="21">
+        <v>0</v>
+      </c>
+      <c r="J13" s="22">
         <v>8.3000000000000007</v>
       </c>
-      <c r="K12" s="21">
-        <v>0</v>
-      </c>
-      <c r="L12" s="22">
-        <v>0</v>
-      </c>
-      <c r="M12" s="21">
+      <c r="K13" s="21">
+        <v>0</v>
+      </c>
+      <c r="L13" s="22">
+        <v>0</v>
+      </c>
+      <c r="M13" s="21">
         <v>8.91</v>
       </c>
-      <c r="N12" s="22">
-        <v>0</v>
-      </c>
-      <c r="O12" s="21">
-        <v>0</v>
-      </c>
-      <c r="P12" s="22">
+      <c r="N13" s="22">
+        <v>0</v>
+      </c>
+      <c r="O13" s="21">
+        <v>0</v>
+      </c>
+      <c r="P13" s="22">
         <v>8.9700000000000006</v>
       </c>
-      <c r="Q12" s="21">
-        <v>0</v>
-      </c>
-      <c r="R12" s="22">
-        <v>0</v>
-      </c>
-      <c r="S12" s="21">
-        <v>0</v>
-      </c>
-      <c r="T12" s="15">
+      <c r="Q13" s="21">
+        <v>0</v>
+      </c>
+      <c r="R13" s="22">
+        <v>0</v>
+      </c>
+      <c r="S13" s="21">
+        <v>0</v>
+      </c>
+      <c r="T13" s="36">
         <f t="shared" si="1"/>
         <v>26.18</v>
       </c>
-      <c r="U12" s="15">
+      <c r="U13" s="36">
         <f t="shared" si="2"/>
         <v>34.380000000000003</v>
       </c>
-      <c r="V12" s="13">
+      <c r="V13" s="37">
         <f t="shared" si="3"/>
         <v>2985.4800000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A13" s="31" t="s">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B14" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D14" s="5">
         <v>36.692999999999998</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E14" s="20">
         <f t="shared" si="0"/>
         <v>40.452129834028291</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F14" s="6">
         <f>'Initial Buys'!E98</f>
         <v>1453.6</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G14" s="15">
         <f>'2015'!S12</f>
         <v>7.26</v>
       </c>
-      <c r="H13" s="22">
-        <v>0</v>
-      </c>
-      <c r="I13" s="21">
-        <v>0</v>
-      </c>
-      <c r="J13" s="22">
-        <v>0</v>
-      </c>
-      <c r="K13" s="21">
+      <c r="H14" s="22">
+        <v>0</v>
+      </c>
+      <c r="I14" s="21">
+        <v>0</v>
+      </c>
+      <c r="J14" s="22">
+        <v>0</v>
+      </c>
+      <c r="K14" s="21">
         <v>7.75</v>
       </c>
-      <c r="L13" s="22">
-        <v>0</v>
-      </c>
-      <c r="M13" s="21">
-        <v>0</v>
-      </c>
-      <c r="N13" s="22">
+      <c r="L14" s="22">
+        <v>0</v>
+      </c>
+      <c r="M14" s="21">
+        <v>0</v>
+      </c>
+      <c r="N14" s="22">
         <v>7.82</v>
       </c>
-      <c r="O13" s="21">
-        <v>0</v>
-      </c>
-      <c r="P13" s="22">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="21">
+      <c r="O14" s="21">
+        <v>0</v>
+      </c>
+      <c r="P14" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="21">
         <v>7.88</v>
       </c>
-      <c r="R13" s="22">
-        <v>0</v>
-      </c>
-      <c r="S13" s="21">
-        <v>0</v>
-      </c>
-      <c r="T13" s="14">
+      <c r="R14" s="22">
+        <v>0</v>
+      </c>
+      <c r="S14" s="21">
+        <v>0</v>
+      </c>
+      <c r="T14" s="15">
         <f t="shared" si="1"/>
         <v>23.45</v>
       </c>
-      <c r="U13" s="14">
+      <c r="U14" s="15">
         <f t="shared" si="2"/>
         <v>30.709999999999997</v>
       </c>
-      <c r="V13" s="12">
+      <c r="V14" s="13">
         <f t="shared" si="3"/>
         <v>1484.31</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A14" s="30" t="s">
+    <row r="15" spans="1:22" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="32">
+        <v>15</v>
+      </c>
+      <c r="E15" s="34">
+        <f t="shared" si="0"/>
+        <v>94.18</v>
+      </c>
+      <c r="F15" s="35">
+        <f>'Initial Buys'!E200</f>
+        <v>1412.7</v>
+      </c>
+      <c r="G15" s="36">
+        <v>0</v>
+      </c>
+      <c r="H15" s="22">
+        <v>0</v>
+      </c>
+      <c r="I15" s="21">
+        <v>0</v>
+      </c>
+      <c r="J15" s="22">
+        <v>0</v>
+      </c>
+      <c r="K15" s="21">
+        <v>0</v>
+      </c>
+      <c r="L15" s="22">
+        <v>0</v>
+      </c>
+      <c r="M15" s="21">
+        <v>0</v>
+      </c>
+      <c r="N15" s="22">
+        <v>0</v>
+      </c>
+      <c r="O15" s="21">
+        <v>0</v>
+      </c>
+      <c r="P15" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="21">
+        <v>0</v>
+      </c>
+      <c r="R15" s="22">
+        <v>0</v>
+      </c>
+      <c r="S15" s="21">
+        <v>0</v>
+      </c>
+      <c r="T15" s="36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U15" s="36">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V15" s="37">
+        <f t="shared" si="3"/>
+        <v>1412.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B16" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D16" s="5">
         <v>7.1879999999999997</v>
       </c>
-      <c r="E14" s="20">
+      <c r="E16" s="20">
         <f t="shared" si="0"/>
         <v>140.40066777963273</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F16" s="6">
         <f>'Initial Buys'!H98</f>
         <v>978.46</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G16" s="15">
         <f>'2015'!S13</f>
         <v>7.18</v>
       </c>
-      <c r="H14" s="22">
-        <v>0</v>
-      </c>
-      <c r="I14" s="21">
-        <v>0</v>
-      </c>
-      <c r="J14" s="22">
+      <c r="H16" s="22">
+        <v>0</v>
+      </c>
+      <c r="I16" s="21">
+        <v>0</v>
+      </c>
+      <c r="J16" s="22">
         <v>7.77</v>
       </c>
-      <c r="K14" s="21">
-        <v>0</v>
-      </c>
-      <c r="L14" s="22">
-        <v>0</v>
-      </c>
-      <c r="M14" s="21">
+      <c r="K16" s="21">
+        <v>0</v>
+      </c>
+      <c r="L16" s="22">
+        <v>0</v>
+      </c>
+      <c r="M16" s="21">
         <v>7.86</v>
       </c>
-      <c r="N14" s="22">
-        <v>0</v>
-      </c>
-      <c r="O14" s="21">
-        <v>0</v>
-      </c>
-      <c r="P14" s="22">
+      <c r="N16" s="22">
+        <v>0</v>
+      </c>
+      <c r="O16" s="21">
+        <v>0</v>
+      </c>
+      <c r="P16" s="22">
         <v>7.93</v>
       </c>
-      <c r="Q14" s="21">
-        <v>0</v>
-      </c>
-      <c r="R14" s="22">
-        <v>0</v>
-      </c>
-      <c r="S14" s="21">
-        <v>0</v>
-      </c>
-      <c r="T14" s="15">
+      <c r="Q16" s="21">
+        <v>0</v>
+      </c>
+      <c r="R16" s="22">
+        <v>0</v>
+      </c>
+      <c r="S16" s="21">
+        <v>0</v>
+      </c>
+      <c r="T16" s="15">
         <f t="shared" si="1"/>
         <v>23.56</v>
       </c>
-      <c r="U14" s="15">
+      <c r="U16" s="15">
         <f t="shared" si="2"/>
         <v>30.74</v>
       </c>
-      <c r="V14" s="13">
+      <c r="V16" s="13">
         <f t="shared" si="3"/>
         <v>1009.2</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A15" s="31" t="s">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B17" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C17" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D17" s="32">
         <v>29.283999999999999</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E17" s="34">
         <f t="shared" si="0"/>
         <v>66.718003005053959</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F17" s="35">
         <f>'Initial Buys'!K98</f>
         <v>1936.08</v>
       </c>
-      <c r="G15" s="14">
-        <v>0</v>
-      </c>
-      <c r="H15" s="22">
-        <v>0</v>
-      </c>
-      <c r="I15" s="21">
-        <v>0</v>
-      </c>
-      <c r="J15" s="22">
-        <v>0</v>
-      </c>
-      <c r="K15" s="21">
-        <v>0</v>
-      </c>
-      <c r="L15" s="22">
-        <v>0</v>
-      </c>
-      <c r="M15" s="21">
-        <v>0</v>
-      </c>
-      <c r="N15" s="22">
-        <v>0</v>
-      </c>
-      <c r="O15" s="21">
-        <v>0</v>
-      </c>
-      <c r="P15" s="22">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="21">
+      <c r="G17" s="36">
+        <v>0</v>
+      </c>
+      <c r="H17" s="22">
+        <v>0</v>
+      </c>
+      <c r="I17" s="21">
+        <v>0</v>
+      </c>
+      <c r="J17" s="22">
+        <v>0</v>
+      </c>
+      <c r="K17" s="21">
+        <v>0</v>
+      </c>
+      <c r="L17" s="22">
+        <v>0</v>
+      </c>
+      <c r="M17" s="21">
+        <v>0</v>
+      </c>
+      <c r="N17" s="22">
+        <v>0</v>
+      </c>
+      <c r="O17" s="21">
+        <v>0</v>
+      </c>
+      <c r="P17" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="21">
         <v>17.690000000000001</v>
       </c>
-      <c r="R15" s="22">
-        <v>0</v>
-      </c>
-      <c r="S15" s="21">
-        <v>0</v>
-      </c>
-      <c r="T15" s="14">
+      <c r="R17" s="22">
+        <v>0</v>
+      </c>
+      <c r="S17" s="21">
+        <v>0</v>
+      </c>
+      <c r="T17" s="36">
         <f t="shared" si="1"/>
         <v>17.690000000000001</v>
       </c>
-      <c r="U15" s="14">
+      <c r="U17" s="36">
         <f t="shared" si="2"/>
         <v>17.690000000000001</v>
       </c>
-      <c r="V15" s="12">
+      <c r="V17" s="37">
         <f t="shared" si="3"/>
         <v>1953.77</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A16" s="30" t="s">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B18" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C18" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D18" s="5">
         <v>4.056</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E18" s="20">
         <f t="shared" si="0"/>
         <v>103.42948717948718</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F18" s="6">
         <f>'Initial Buys'!N98</f>
         <v>413.52</v>
       </c>
-      <c r="G16" s="15">
-        <v>0</v>
-      </c>
-      <c r="H16" s="22">
-        <v>0</v>
-      </c>
-      <c r="I16" s="21">
-        <v>0</v>
-      </c>
-      <c r="J16" s="22">
-        <v>0</v>
-      </c>
-      <c r="K16" s="21">
-        <v>0</v>
-      </c>
-      <c r="L16" s="22">
-        <v>0</v>
-      </c>
-      <c r="M16" s="21">
+      <c r="G18" s="15">
+        <v>0</v>
+      </c>
+      <c r="H18" s="22">
+        <v>0</v>
+      </c>
+      <c r="I18" s="21">
+        <v>0</v>
+      </c>
+      <c r="J18" s="22">
+        <v>0</v>
+      </c>
+      <c r="K18" s="21">
+        <v>0</v>
+      </c>
+      <c r="L18" s="22">
+        <v>0</v>
+      </c>
+      <c r="M18" s="21">
         <v>2.96</v>
       </c>
-      <c r="N16" s="22">
-        <v>0</v>
-      </c>
-      <c r="O16" s="21">
-        <v>0</v>
-      </c>
-      <c r="P16" s="22">
+      <c r="N18" s="22">
+        <v>0</v>
+      </c>
+      <c r="O18" s="21">
+        <v>0</v>
+      </c>
+      <c r="P18" s="22">
         <v>3.03</v>
       </c>
-      <c r="Q16" s="21">
-        <v>0</v>
-      </c>
-      <c r="R16" s="22">
-        <v>0</v>
-      </c>
-      <c r="S16" s="21">
-        <v>0</v>
-      </c>
-      <c r="T16" s="15">
+      <c r="Q18" s="21">
+        <v>0</v>
+      </c>
+      <c r="R18" s="22">
+        <v>0</v>
+      </c>
+      <c r="S18" s="21">
+        <v>0</v>
+      </c>
+      <c r="T18" s="15">
         <f t="shared" si="1"/>
         <v>5.99</v>
       </c>
-      <c r="U16" s="15">
+      <c r="U18" s="15">
         <f t="shared" si="2"/>
         <v>5.99</v>
       </c>
-      <c r="V16" s="13">
+      <c r="V18" s="13">
         <f t="shared" si="3"/>
         <v>419.51</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A17" s="31" t="s">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B19" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C19" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D19" s="32">
         <v>25.466000000000001</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E19" s="34">
         <f t="shared" si="0"/>
         <v>77.880311002905827</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F19" s="35">
         <f>'Initial Buys'!Q98</f>
         <v>1945.52</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G19" s="36">
         <f>'2015'!S14</f>
         <v>9.2799999999999994</v>
       </c>
-      <c r="H17" s="22">
-        <v>0</v>
-      </c>
-      <c r="I17" s="21">
+      <c r="H19" s="22">
+        <v>0</v>
+      </c>
+      <c r="I19" s="21">
         <v>9.36</v>
       </c>
-      <c r="J17" s="22">
-        <v>0</v>
-      </c>
-      <c r="K17" s="21">
-        <v>0</v>
-      </c>
-      <c r="L17" s="22">
+      <c r="J19" s="22">
+        <v>0</v>
+      </c>
+      <c r="K19" s="21">
+        <v>0</v>
+      </c>
+      <c r="L19" s="22">
         <v>9.5299999999999994</v>
       </c>
-      <c r="M17" s="21">
-        <v>0</v>
-      </c>
-      <c r="N17" s="22">
-        <v>0</v>
-      </c>
-      <c r="O17" s="21">
+      <c r="M19" s="21">
+        <v>0</v>
+      </c>
+      <c r="N19" s="22">
+        <v>0</v>
+      </c>
+      <c r="O19" s="21">
         <v>9.61</v>
       </c>
-      <c r="P17" s="22">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="21">
-        <v>0</v>
-      </c>
-      <c r="R17" s="22">
-        <v>0</v>
-      </c>
-      <c r="S17" s="21">
-        <v>0</v>
-      </c>
-      <c r="T17" s="14">
+      <c r="P19" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="21">
+        <v>0</v>
+      </c>
+      <c r="R19" s="22">
+        <v>0</v>
+      </c>
+      <c r="S19" s="21">
+        <v>0</v>
+      </c>
+      <c r="T19" s="36">
         <f t="shared" si="1"/>
         <v>28.5</v>
       </c>
-      <c r="U17" s="14">
+      <c r="U19" s="36">
         <f t="shared" si="2"/>
         <v>37.78</v>
       </c>
-      <c r="V17" s="12">
+      <c r="V19" s="37">
         <f t="shared" si="3"/>
         <v>1983.3</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A18" s="30" t="s">
+    <row r="20" spans="1:22" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="5">
+        <v>10</v>
+      </c>
+      <c r="E20" s="20">
+        <f t="shared" si="0"/>
+        <v>130.34</v>
+      </c>
+      <c r="F20" s="6">
+        <f>'Initial Buys'!H200</f>
+        <v>1303.4000000000001</v>
+      </c>
+      <c r="G20" s="15">
+        <v>0</v>
+      </c>
+      <c r="H20" s="22">
+        <v>0</v>
+      </c>
+      <c r="I20" s="21">
+        <v>0</v>
+      </c>
+      <c r="J20" s="22">
+        <v>0</v>
+      </c>
+      <c r="K20" s="21">
+        <v>0</v>
+      </c>
+      <c r="L20" s="22">
+        <v>0</v>
+      </c>
+      <c r="M20" s="21">
+        <v>0</v>
+      </c>
+      <c r="N20" s="22">
+        <v>0</v>
+      </c>
+      <c r="O20" s="21">
+        <v>0</v>
+      </c>
+      <c r="P20" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="21">
+        <v>0</v>
+      </c>
+      <c r="R20" s="22">
+        <v>0</v>
+      </c>
+      <c r="S20" s="21">
+        <v>0</v>
+      </c>
+      <c r="T20" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U20" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V20" s="13">
+        <f t="shared" si="3"/>
+        <v>1303.4000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B21" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C21" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D21" s="32">
         <v>23.007000000000001</v>
       </c>
-      <c r="E18" s="20">
+      <c r="E21" s="34">
         <f t="shared" si="0"/>
         <v>43.980527665493106</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F21" s="35">
         <f>'Initial Buys'!T98</f>
         <v>962.5</v>
       </c>
-      <c r="G18" s="15">
+      <c r="G21" s="36">
         <f>'2015'!S15</f>
         <v>11.94</v>
       </c>
-      <c r="H18" s="22">
-        <v>0</v>
-      </c>
-      <c r="I18" s="21">
-        <v>0</v>
-      </c>
-      <c r="J18" s="22">
+      <c r="H21" s="22">
+        <v>0</v>
+      </c>
+      <c r="I21" s="21">
+        <v>0</v>
+      </c>
+      <c r="J21" s="22">
         <v>12.08</v>
       </c>
-      <c r="K18" s="21">
-        <v>0</v>
-      </c>
-      <c r="L18" s="22">
-        <v>0</v>
-      </c>
-      <c r="M18" s="21">
+      <c r="K21" s="21">
+        <v>0</v>
+      </c>
+      <c r="L21" s="22">
+        <v>0</v>
+      </c>
+      <c r="M21" s="21">
         <v>12.61</v>
       </c>
-      <c r="N18" s="22">
-        <v>0</v>
-      </c>
-      <c r="O18" s="21">
-        <v>0</v>
-      </c>
-      <c r="P18" s="22">
+      <c r="N21" s="22">
+        <v>0</v>
+      </c>
+      <c r="O21" s="21">
+        <v>0</v>
+      </c>
+      <c r="P21" s="22">
         <v>12.73</v>
       </c>
-      <c r="Q18" s="21">
-        <v>0</v>
-      </c>
-      <c r="R18" s="22">
-        <v>0</v>
-      </c>
-      <c r="S18" s="21">
-        <v>0</v>
-      </c>
-      <c r="T18" s="15">
+      <c r="Q21" s="21">
+        <v>0</v>
+      </c>
+      <c r="R21" s="22">
+        <v>0</v>
+      </c>
+      <c r="S21" s="21">
+        <v>0</v>
+      </c>
+      <c r="T21" s="36">
         <f t="shared" si="1"/>
         <v>37.42</v>
       </c>
-      <c r="U18" s="15">
+      <c r="U21" s="36">
         <f t="shared" si="2"/>
         <v>49.36</v>
       </c>
-      <c r="V18" s="13">
+      <c r="V21" s="37">
         <f t="shared" si="3"/>
         <v>1011.86</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A19" s="31" t="s">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B22" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C22" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="24">
+      <c r="D22" s="5">
         <v>60.432000000000002</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E22" s="20">
         <f t="shared" si="0"/>
         <v>36.65855837966641</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F22" s="6">
         <f>'Initial Buys'!W98</f>
         <v>2161.0100000000002</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G22" s="15">
         <f>'2015'!S16</f>
         <v>10.15</v>
       </c>
-      <c r="H19" s="22">
-        <v>0</v>
-      </c>
-      <c r="I19" s="21">
+      <c r="H22" s="22">
+        <v>0</v>
+      </c>
+      <c r="I22" s="21">
         <v>14.54</v>
       </c>
-      <c r="J19" s="22">
-        <v>0</v>
-      </c>
-      <c r="K19" s="21">
-        <v>0</v>
-      </c>
-      <c r="L19" s="22">
+      <c r="J22" s="22">
+        <v>0</v>
+      </c>
+      <c r="K22" s="21">
+        <v>0</v>
+      </c>
+      <c r="L22" s="22">
         <v>14.73</v>
       </c>
-      <c r="M19" s="21">
-        <v>0</v>
-      </c>
-      <c r="N19" s="22">
-        <v>0</v>
-      </c>
-      <c r="O19" s="21">
+      <c r="M22" s="21">
+        <v>0</v>
+      </c>
+      <c r="N22" s="22">
+        <v>0</v>
+      </c>
+      <c r="O22" s="21">
         <v>14.92</v>
       </c>
-      <c r="P19" s="22">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="21">
-        <v>0</v>
-      </c>
-      <c r="R19" s="22">
-        <v>0</v>
-      </c>
-      <c r="S19" s="21">
-        <v>0</v>
-      </c>
-      <c r="T19" s="14">
+      <c r="P22" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="21">
+        <v>0</v>
+      </c>
+      <c r="R22" s="22">
+        <v>0</v>
+      </c>
+      <c r="S22" s="21">
+        <v>0</v>
+      </c>
+      <c r="T22" s="15">
         <f t="shared" si="1"/>
         <v>44.19</v>
       </c>
-      <c r="U19" s="14">
+      <c r="U22" s="15">
         <f t="shared" si="2"/>
         <v>54.34</v>
       </c>
-      <c r="V19" s="12">
+      <c r="V22" s="13">
         <f t="shared" si="3"/>
         <v>2215.3500000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A20" s="30" t="s">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B23" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C23" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D23" s="32">
         <v>34.156999999999996</v>
       </c>
-      <c r="E20" s="20">
+      <c r="E23" s="34">
         <f t="shared" si="0"/>
         <v>51.696577568287616</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F23" s="35">
         <f>'Initial Buys'!Z98</f>
         <v>1757.33</v>
       </c>
-      <c r="G20" s="15">
-        <v>0</v>
-      </c>
-      <c r="H20" s="22">
-        <v>0</v>
-      </c>
-      <c r="I20" s="21">
-        <v>0</v>
-      </c>
-      <c r="J20" s="22">
-        <v>0</v>
-      </c>
-      <c r="K20" s="21">
-        <v>0</v>
-      </c>
-      <c r="L20" s="22">
-        <v>0</v>
-      </c>
-      <c r="M20" s="21">
-        <v>0</v>
-      </c>
-      <c r="N20" s="22">
-        <v>0</v>
-      </c>
-      <c r="O20" s="21">
+      <c r="G23" s="36">
+        <v>0</v>
+      </c>
+      <c r="H23" s="22">
+        <v>0</v>
+      </c>
+      <c r="I23" s="21">
+        <v>0</v>
+      </c>
+      <c r="J23" s="22">
+        <v>0</v>
+      </c>
+      <c r="K23" s="21">
+        <v>0</v>
+      </c>
+      <c r="L23" s="22">
+        <v>0</v>
+      </c>
+      <c r="M23" s="21">
+        <v>0</v>
+      </c>
+      <c r="N23" s="22">
+        <v>0</v>
+      </c>
+      <c r="O23" s="21">
         <v>8.4700000000000006</v>
       </c>
-      <c r="P20" s="22">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="21">
-        <v>0</v>
-      </c>
-      <c r="R20" s="22">
-        <v>0</v>
-      </c>
-      <c r="S20" s="21">
-        <v>0</v>
-      </c>
-      <c r="T20" s="15">
+      <c r="P23" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="21">
+        <v>0</v>
+      </c>
+      <c r="R23" s="22">
+        <v>0</v>
+      </c>
+      <c r="S23" s="21">
+        <v>0</v>
+      </c>
+      <c r="T23" s="36">
         <f t="shared" si="1"/>
         <v>8.4700000000000006</v>
       </c>
-      <c r="U20" s="15">
+      <c r="U23" s="36">
         <f t="shared" si="2"/>
         <v>8.4700000000000006</v>
       </c>
-      <c r="V20" s="13">
+      <c r="V23" s="37">
         <f t="shared" si="3"/>
         <v>1765.8</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A21" s="31" t="s">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B24" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C24" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="24">
+      <c r="D24" s="5">
         <v>29.777000000000001</v>
       </c>
-      <c r="E21" s="19">
+      <c r="E24" s="20">
         <f t="shared" si="0"/>
         <v>66.146018739295428</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F24" s="6">
         <f>'Initial Buys'!AC98</f>
         <v>1916.7600000000002</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G24" s="15">
         <f>'2015'!S17</f>
         <v>0</v>
       </c>
-      <c r="H21" s="22">
+      <c r="H24" s="22">
         <v>14.67</v>
       </c>
-      <c r="I21" s="21">
-        <v>0</v>
-      </c>
-      <c r="J21" s="22">
-        <v>0</v>
-      </c>
-      <c r="K21" s="21">
+      <c r="I24" s="21">
+        <v>0</v>
+      </c>
+      <c r="J24" s="22">
+        <v>0</v>
+      </c>
+      <c r="K24" s="21">
         <v>15.15</v>
       </c>
-      <c r="L21" s="22">
-        <v>0</v>
-      </c>
-      <c r="M21" s="21">
+      <c r="L24" s="22">
+        <v>0</v>
+      </c>
+      <c r="M24" s="21">
         <v>15.23</v>
       </c>
-      <c r="N21" s="22">
-        <v>0</v>
-      </c>
-      <c r="O21" s="21">
-        <v>0</v>
-      </c>
-      <c r="P21" s="22">
+      <c r="N24" s="22">
+        <v>0</v>
+      </c>
+      <c r="O24" s="21">
+        <v>0</v>
+      </c>
+      <c r="P24" s="22">
         <v>7.82</v>
       </c>
-      <c r="Q21" s="21">
-        <v>0</v>
-      </c>
-      <c r="R21" s="22">
-        <v>0</v>
-      </c>
-      <c r="S21" s="21">
-        <v>0</v>
-      </c>
-      <c r="T21" s="14">
+      <c r="Q24" s="21">
+        <v>0</v>
+      </c>
+      <c r="R24" s="22">
+        <v>0</v>
+      </c>
+      <c r="S24" s="21">
+        <v>0</v>
+      </c>
+      <c r="T24" s="15">
         <f t="shared" si="1"/>
         <v>52.87</v>
       </c>
-      <c r="U21" s="14">
+      <c r="U24" s="15">
         <f t="shared" si="2"/>
         <v>52.87</v>
       </c>
-      <c r="V21" s="12">
+      <c r="V24" s="13">
         <f t="shared" si="3"/>
         <v>1969.63</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A22" s="30" t="s">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B25" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C25" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D25" s="32">
         <v>25.503</v>
       </c>
-      <c r="E22" s="20">
+      <c r="E25" s="34">
         <f t="shared" si="0"/>
         <v>79.626710583068657</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F25" s="35">
         <f>'Initial Buys'!B148</f>
         <v>1988.76</v>
       </c>
-      <c r="G22" s="15">
+      <c r="G25" s="36">
         <f>'2015'!S18</f>
         <v>10.18</v>
       </c>
-      <c r="H22" s="22">
-        <v>0</v>
-      </c>
-      <c r="I22" s="21">
-        <v>0</v>
-      </c>
-      <c r="J22" s="22">
+      <c r="H25" s="22">
+        <v>0</v>
+      </c>
+      <c r="I25" s="21">
+        <v>0</v>
+      </c>
+      <c r="J25" s="22">
         <v>10.3</v>
       </c>
-      <c r="K22" s="21">
-        <v>0</v>
-      </c>
-      <c r="L22" s="22">
-        <v>0</v>
-      </c>
-      <c r="M22" s="21">
+      <c r="K25" s="21">
+        <v>0</v>
+      </c>
+      <c r="L25" s="22">
+        <v>0</v>
+      </c>
+      <c r="M25" s="21">
         <v>10.7</v>
       </c>
-      <c r="N22" s="22">
-        <v>0</v>
-      </c>
-      <c r="O22" s="21">
-        <v>0</v>
-      </c>
-      <c r="P22" s="22">
+      <c r="N25" s="22">
+        <v>0</v>
+      </c>
+      <c r="O25" s="21">
+        <v>0</v>
+      </c>
+      <c r="P25" s="22">
         <v>10.78</v>
       </c>
-      <c r="Q22" s="21">
-        <v>0</v>
-      </c>
-      <c r="R22" s="22">
-        <v>0</v>
-      </c>
-      <c r="S22" s="21">
-        <v>0</v>
-      </c>
-      <c r="T22" s="15">
+      <c r="Q25" s="21">
+        <v>0</v>
+      </c>
+      <c r="R25" s="22">
+        <v>0</v>
+      </c>
+      <c r="S25" s="21">
+        <v>0</v>
+      </c>
+      <c r="T25" s="36">
         <f t="shared" si="1"/>
         <v>31.78</v>
       </c>
-      <c r="U22" s="15">
+      <c r="U25" s="36">
         <f t="shared" si="2"/>
         <v>41.96</v>
       </c>
-      <c r="V22" s="13">
+      <c r="V25" s="37">
         <f t="shared" si="3"/>
         <v>2030.72</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="27">
-        <f>SUM(G2:G22)</f>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="27">
+        <f>SUM(G2:G25)</f>
         <v>134.23000000000002</v>
       </c>
-      <c r="H23" s="16">
-        <f>SUM(H2:H22)</f>
+      <c r="H26" s="16">
+        <f>SUM(H2:H25)</f>
         <v>21.3</v>
       </c>
-      <c r="I23" s="27">
-        <f t="shared" ref="I23:U23" si="4">SUM(I2:I22)</f>
+      <c r="I26" s="27">
+        <f t="shared" ref="I26:U26" si="4">SUM(I2:I25)</f>
         <v>58.78</v>
       </c>
-      <c r="J23" s="16">
+      <c r="J26" s="16">
         <f t="shared" si="4"/>
         <v>80.88</v>
       </c>
-      <c r="K23" s="27">
+      <c r="K26" s="27">
         <f t="shared" si="4"/>
         <v>29.560000000000002</v>
       </c>
-      <c r="L23" s="16">
+      <c r="L26" s="16">
         <f t="shared" si="4"/>
         <v>60</v>
       </c>
-      <c r="M23" s="27">
+      <c r="M26" s="27">
         <f t="shared" si="4"/>
         <v>101.09</v>
       </c>
-      <c r="N23" s="16">
+      <c r="N26" s="16">
         <f t="shared" si="4"/>
         <v>14.530000000000001</v>
       </c>
-      <c r="O23" s="27">
+      <c r="O26" s="27">
         <f t="shared" si="4"/>
         <v>69.400000000000006</v>
       </c>
-      <c r="P23" s="16">
+      <c r="P26" s="16">
         <f t="shared" si="4"/>
         <v>94.43</v>
       </c>
-      <c r="Q23" s="27">
+      <c r="Q26" s="27">
         <f t="shared" si="4"/>
         <v>35.24</v>
       </c>
-      <c r="R23" s="16">
+      <c r="R26" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="S23" s="27">
+      <c r="S26" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T23" s="27">
+      <c r="T26" s="27">
         <f t="shared" si="4"/>
         <v>565.21</v>
       </c>
-      <c r="U23" s="27">
+      <c r="U26" s="27">
         <f t="shared" si="4"/>
         <v>699.44</v>
       </c>
-      <c r="V23" s="18">
-        <f>SUM(V2:V22)</f>
-        <v>30095.21</v>
+      <c r="V26" s="18">
+        <f>SUM(V2:V25)</f>
+        <v>34853.810000000005</v>
       </c>
     </row>
   </sheetData>
@@ -4813,31 +5090,31 @@
       <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -4905,7 +5182,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
@@ -4979,7 +5256,7 @@
         <v>1069.8499999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>21</v>
       </c>
@@ -5053,7 +5330,7 @@
         <v>1853.59</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
@@ -5127,7 +5404,7 @@
         <v>1076.93</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>23</v>
       </c>
@@ -5149,7 +5426,7 @@
         <v>1013.44</v>
       </c>
       <c r="G5" s="14">
-        <f>'2016'!U5</f>
+        <f>'2016'!U6</f>
         <v>24.810000000000002</v>
       </c>
       <c r="H5" s="22">
@@ -5201,7 +5478,7 @@
         <v>1038.25</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -5223,7 +5500,7 @@
         <v>1072.4000000000001</v>
       </c>
       <c r="G6" s="15">
-        <f>'2016'!U6</f>
+        <f>'2016'!U7</f>
         <v>60.89</v>
       </c>
       <c r="H6" s="22">
@@ -5275,7 +5552,7 @@
         <v>1133.2900000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>25</v>
       </c>
@@ -5297,7 +5574,7 @@
         <v>1012.94</v>
       </c>
       <c r="G7" s="14">
-        <f>'2016'!U7</f>
+        <f>'2016'!U8</f>
         <v>25.4</v>
       </c>
       <c r="H7" s="22">
@@ -5349,7 +5626,7 @@
         <v>1038.3400000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>26</v>
       </c>
@@ -5371,7 +5648,7 @@
         <v>920.78</v>
       </c>
       <c r="G8" s="15">
-        <f>'2016'!U8</f>
+        <f>'2016'!U9</f>
         <v>37.699999999999996</v>
       </c>
       <c r="H8" s="22">
@@ -5423,7 +5700,7 @@
         <v>958.48</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>7</v>
       </c>
@@ -5445,7 +5722,7 @@
         <v>997.04</v>
       </c>
       <c r="G9" s="14">
-        <f>'2016'!U9</f>
+        <f>'2016'!U10</f>
         <v>42.4</v>
       </c>
       <c r="H9" s="22">
@@ -5497,7 +5774,7 @@
         <v>1039.44</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
@@ -5519,7 +5796,7 @@
         <v>1027.08</v>
       </c>
       <c r="G10" s="15">
-        <f>'2016'!U10</f>
+        <f>'2016'!U11</f>
         <v>30.86</v>
       </c>
       <c r="H10" s="22">
@@ -5571,7 +5848,7 @@
         <v>1057.9399999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>28</v>
       </c>
@@ -5593,7 +5870,7 @@
         <v>989.4</v>
       </c>
       <c r="G11" s="14">
-        <f>'2016'!U11</f>
+        <f>'2016'!U12</f>
         <v>32.72</v>
       </c>
       <c r="H11" s="22">
@@ -5645,7 +5922,7 @@
         <v>1022.12</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
@@ -5667,7 +5944,7 @@
         <v>2951.1000000000004</v>
       </c>
       <c r="G12" s="15">
-        <f>'2016'!U12</f>
+        <f>'2016'!U13</f>
         <v>34.380000000000003</v>
       </c>
       <c r="H12" s="22">
@@ -5719,7 +5996,7 @@
         <v>2985.4800000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>17</v>
       </c>
@@ -5741,7 +6018,7 @@
         <v>1453.6</v>
       </c>
       <c r="G13" s="14">
-        <f>'2016'!U13</f>
+        <f>'2016'!U14</f>
         <v>30.709999999999997</v>
       </c>
       <c r="H13" s="22">
@@ -5793,7 +6070,7 @@
         <v>1484.31</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>29</v>
       </c>
@@ -5815,7 +6092,7 @@
         <v>978.46</v>
       </c>
       <c r="G14" s="15">
-        <f>'2016'!U14</f>
+        <f>'2016'!U16</f>
         <v>30.74</v>
       </c>
       <c r="H14" s="22">
@@ -5867,7 +6144,7 @@
         <v>1009.2</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>30</v>
       </c>
@@ -5889,7 +6166,7 @@
         <v>1936.08</v>
       </c>
       <c r="G15" s="14">
-        <f>'2016'!U15</f>
+        <f>'2016'!U17</f>
         <v>17.690000000000001</v>
       </c>
       <c r="H15" s="22">
@@ -5941,7 +6218,7 @@
         <v>1953.77</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>31</v>
       </c>
@@ -5963,7 +6240,7 @@
         <v>413.52</v>
       </c>
       <c r="G16" s="15">
-        <f>'2016'!U16</f>
+        <f>'2016'!U18</f>
         <v>5.99</v>
       </c>
       <c r="H16" s="22">
@@ -6015,7 +6292,7 @@
         <v>422.46999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>32</v>
       </c>
@@ -6037,7 +6314,7 @@
         <v>1945.52</v>
       </c>
       <c r="G17" s="14">
-        <f>'2016'!U17</f>
+        <f>'2016'!U19</f>
         <v>37.78</v>
       </c>
       <c r="H17" s="22">
@@ -6089,7 +6366,7 @@
         <v>1983.3</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>33</v>
       </c>
@@ -6111,7 +6388,7 @@
         <v>962.5</v>
       </c>
       <c r="G18" s="15">
-        <f>'2016'!U18</f>
+        <f>'2016'!U21</f>
         <v>49.36</v>
       </c>
       <c r="H18" s="22">
@@ -6163,7 +6440,7 @@
         <v>1011.86</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>34</v>
       </c>
@@ -6185,7 +6462,7 @@
         <v>2161.0100000000002</v>
       </c>
       <c r="G19" s="14">
-        <f>'2016'!U19</f>
+        <f>'2016'!U22</f>
         <v>54.34</v>
       </c>
       <c r="H19" s="22">
@@ -6237,7 +6514,7 @@
         <v>2215.3500000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>36</v>
       </c>
@@ -6259,7 +6536,7 @@
         <v>1757.33</v>
       </c>
       <c r="G20" s="15">
-        <f>'2016'!U20</f>
+        <f>'2016'!U23</f>
         <v>8.4700000000000006</v>
       </c>
       <c r="H20" s="22">
@@ -6311,7 +6588,7 @@
         <v>1765.8</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>37</v>
       </c>
@@ -6333,7 +6610,7 @@
         <v>1916.7600000000002</v>
       </c>
       <c r="G21" s="14">
-        <f>'2016'!U21</f>
+        <f>'2016'!U24</f>
         <v>52.87</v>
       </c>
       <c r="H21" s="22">
@@ -6385,7 +6662,7 @@
         <v>1969.63</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>38</v>
       </c>
@@ -6407,7 +6684,7 @@
         <v>1988.76</v>
       </c>
       <c r="G22" s="15">
-        <f>'2016'!U22</f>
+        <f>'2016'!U25</f>
         <v>41.96</v>
       </c>
       <c r="H22" s="22">
@@ -6459,7 +6736,7 @@
         <v>2030.72</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="26"/>
       <c r="B23" s="26"/>
       <c r="C23" s="26"/>

</xml_diff>